<commit_message>
Draft 1 - CHI note
</commit_message>
<xml_diff>
--- a/Docs/Post-Experiment Questionarie.xlsx
+++ b/Docs/Post-Experiment Questionarie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Likert Questions" sheetId="1" r:id="rId1"/>
@@ -610,11 +610,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104905344"/>
-        <c:axId val="104911232"/>
+        <c:axId val="120240768"/>
+        <c:axId val="120246656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104905344"/>
+        <c:axId val="120240768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,7 +623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104911232"/>
+        <c:crossAx val="120246656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -631,7 +631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104911232"/>
+        <c:axId val="120246656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,7 +642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104905344"/>
+        <c:crossAx val="120240768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -873,11 +873,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104964096"/>
-        <c:axId val="104965632"/>
+        <c:axId val="121544704"/>
+        <c:axId val="121546240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104964096"/>
+        <c:axId val="121544704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104965632"/>
+        <c:crossAx val="121546240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -894,7 +894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104965632"/>
+        <c:axId val="121546240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104964096"/>
+        <c:crossAx val="121544704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,11 +1136,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="118182656"/>
-        <c:axId val="118184192"/>
+        <c:axId val="121721600"/>
+        <c:axId val="121723136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118182656"/>
+        <c:axId val="121721600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118184192"/>
+        <c:crossAx val="121723136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1157,7 +1157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118184192"/>
+        <c:axId val="121723136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118182656"/>
+        <c:crossAx val="121721600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1241,6 +1241,22 @@
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$26:$AB$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.9885947395720818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8122650608345792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2440710539815454</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7440710539815454</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1276,6 +1292,22 @@
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$27:$AB$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1311,6 +1343,22 @@
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$28:$AB$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1346,6 +1394,22 @@
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$29:$AB$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1380,6 +1444,22 @@
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$30:$AB$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.7614052604279182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1877349391654208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7559289460184546</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2559289460184546</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1400,11 +1480,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119541760"/>
-        <c:axId val="119543296"/>
+        <c:axId val="121763328"/>
+        <c:axId val="121764864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119541760"/>
+        <c:axId val="121763328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119543296"/>
+        <c:crossAx val="121764864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119543296"/>
+        <c:axId val="121764864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119541760"/>
+        <c:crossAx val="121763328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1500,27 +1580,26 @@
           <c:cat>
             <c:strRef>
               <c:f>'Likert Questions'!$Y$33:$AB$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No Camera</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Mask</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mask</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$34:$AB$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5422620262886748</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0741799002274486</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1906926585840458</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1551,27 +1630,26 @@
           <c:cat>
             <c:strRef>
               <c:f>'Likert Questions'!$Y$33:$AB$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No Camera</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Mask</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mask</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$35:$AB$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1602,27 +1680,26 @@
           <c:cat>
             <c:strRef>
               <c:f>'Likert Questions'!$Y$33:$AB$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No Camera</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Mask</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mask</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$36:$AB$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1653,27 +1730,26 @@
           <c:cat>
             <c:strRef>
               <c:f>'Likert Questions'!$Y$33:$AB$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No Camera</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Mask</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mask</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$37:$AB$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1703,27 +1779,26 @@
           <c:cat>
             <c:strRef>
               <c:f>'Likert Questions'!$Y$33:$AB$33</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No Camera</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Camera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>No Mask</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mask</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Likert Questions'!$Y$38:$AB$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4577379737113247</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.925820099772551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8093073414159537</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1743,11 +1818,11 @@
         </c:upDownBars>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119587584"/>
-        <c:axId val="119589120"/>
+        <c:axId val="121827328"/>
+        <c:axId val="121828864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119587584"/>
+        <c:axId val="121827328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119589120"/>
+        <c:crossAx val="121828864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1764,7 +1839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119589120"/>
+        <c:axId val="121828864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,355 +1850,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119587584"/>
+        <c:crossAx val="121827328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Likert Questions'!$X$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>q1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Likert Questions'!$Y$41:$AB$41</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>No Camera</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Camera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>No Mask</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mask</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Likert Questions'!$Y$42:$AB$42</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Likert Questions'!$X$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>min</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="dash"/>
-            <c:size val="7"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Likert Questions'!$Y$41:$AB$41</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>No Camera</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Camera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>No Mask</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mask</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Likert Questions'!$Y$43:$AB$43</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Likert Questions'!$X$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>average</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="dash"/>
-            <c:size val="7"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Likert Questions'!$Y$41:$AB$41</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>No Camera</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Camera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>No Mask</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mask</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Likert Questions'!$Y$44:$AB$44</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Likert Questions'!$X$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>max</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="dash"/>
-            <c:size val="7"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Likert Questions'!$Y$41:$AB$41</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>No Camera</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Camera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>No Mask</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mask</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Likert Questions'!$Y$45:$AB$45</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Likert Questions'!$X$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>q3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Likert Questions'!$Y$41:$AB$41</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>No Camera</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Camera</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>No Mask</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Mask</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Likert Questions'!$Y$46:$AB$46</c:f>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:upDownBars>
-          <c:gapWidth val="150"/>
-          <c:upBars/>
-          <c:downBars/>
-        </c:upDownBars>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="119625600"/>
-        <c:axId val="119627136"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="119625600"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119627136"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="119627136"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119625600"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2290,36 +2024,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3737,295 +3441,14 @@
 </a:themeOverride>
 </file>
 
-<file path=xl/theme/themeOverride5.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <a:clrScheme name="Office">
-    <a:dk1>
-      <a:sysClr val="windowText" lastClr="000000"/>
-    </a:dk1>
-    <a:lt1>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
-    </a:lt1>
-    <a:dk2>
-      <a:srgbClr val="1F497D"/>
-    </a:dk2>
-    <a:lt2>
-      <a:srgbClr val="EEECE1"/>
-    </a:lt2>
-    <a:accent1>
-      <a:srgbClr val="4F81BD"/>
-    </a:accent1>
-    <a:accent2>
-      <a:srgbClr val="C0504D"/>
-    </a:accent2>
-    <a:accent3>
-      <a:srgbClr val="9BBB59"/>
-    </a:accent3>
-    <a:accent4>
-      <a:srgbClr val="8064A2"/>
-    </a:accent4>
-    <a:accent5>
-      <a:srgbClr val="4BACC6"/>
-    </a:accent5>
-    <a:accent6>
-      <a:srgbClr val="F79646"/>
-    </a:accent6>
-    <a:hlink>
-      <a:srgbClr val="0000FF"/>
-    </a:hlink>
-    <a:folHlink>
-      <a:srgbClr val="800080"/>
-    </a:folHlink>
-  </a:clrScheme>
-  <a:fontScheme name="Office">
-    <a:majorFont>
-      <a:latin typeface="Cambria"/>
-      <a:ea typeface=""/>
-      <a:cs typeface=""/>
-      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-      <a:font script="Hang" typeface="맑은 고딕"/>
-      <a:font script="Hans" typeface="宋体"/>
-      <a:font script="Hant" typeface="新細明體"/>
-      <a:font script="Arab" typeface="Times New Roman"/>
-      <a:font script="Hebr" typeface="Times New Roman"/>
-      <a:font script="Thai" typeface="Tahoma"/>
-      <a:font script="Ethi" typeface="Nyala"/>
-      <a:font script="Beng" typeface="Vrinda"/>
-      <a:font script="Gujr" typeface="Shruti"/>
-      <a:font script="Khmr" typeface="MoolBoran"/>
-      <a:font script="Knda" typeface="Tunga"/>
-      <a:font script="Guru" typeface="Raavi"/>
-      <a:font script="Cans" typeface="Euphemia"/>
-      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-      <a:font script="Thaa" typeface="MV Boli"/>
-      <a:font script="Deva" typeface="Mangal"/>
-      <a:font script="Telu" typeface="Gautami"/>
-      <a:font script="Taml" typeface="Latha"/>
-      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-      <a:font script="Orya" typeface="Kalinga"/>
-      <a:font script="Mlym" typeface="Kartika"/>
-      <a:font script="Laoo" typeface="DokChampa"/>
-      <a:font script="Sinh" typeface="Iskoola Pota"/>
-      <a:font script="Mong" typeface="Mongolian Baiti"/>
-      <a:font script="Viet" typeface="Times New Roman"/>
-      <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      <a:font script="Geor" typeface="Sylfaen"/>
-    </a:majorFont>
-    <a:minorFont>
-      <a:latin typeface="Calibri"/>
-      <a:ea typeface=""/>
-      <a:cs typeface=""/>
-      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-      <a:font script="Hang" typeface="맑은 고딕"/>
-      <a:font script="Hans" typeface="宋体"/>
-      <a:font script="Hant" typeface="新細明體"/>
-      <a:font script="Arab" typeface="Arial"/>
-      <a:font script="Hebr" typeface="Arial"/>
-      <a:font script="Thai" typeface="Tahoma"/>
-      <a:font script="Ethi" typeface="Nyala"/>
-      <a:font script="Beng" typeface="Vrinda"/>
-      <a:font script="Gujr" typeface="Shruti"/>
-      <a:font script="Khmr" typeface="DaunPenh"/>
-      <a:font script="Knda" typeface="Tunga"/>
-      <a:font script="Guru" typeface="Raavi"/>
-      <a:font script="Cans" typeface="Euphemia"/>
-      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-      <a:font script="Thaa" typeface="MV Boli"/>
-      <a:font script="Deva" typeface="Mangal"/>
-      <a:font script="Telu" typeface="Gautami"/>
-      <a:font script="Taml" typeface="Latha"/>
-      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-      <a:font script="Orya" typeface="Kalinga"/>
-      <a:font script="Mlym" typeface="Kartika"/>
-      <a:font script="Laoo" typeface="DokChampa"/>
-      <a:font script="Sinh" typeface="Iskoola Pota"/>
-      <a:font script="Mong" typeface="Mongolian Baiti"/>
-      <a:font script="Viet" typeface="Arial"/>
-      <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      <a:font script="Geor" typeface="Sylfaen"/>
-    </a:minorFont>
-  </a:fontScheme>
-  <a:fmtScheme name="Office">
-    <a:fillStyleLst>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:tint val="50000"/>
-              <a:satMod val="300000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="35000">
-            <a:schemeClr val="phClr">
-              <a:tint val="37000"/>
-              <a:satMod val="300000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:tint val="15000"/>
-              <a:satMod val="350000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="16200000" scaled="1"/>
-      </a:gradFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:shade val="51000"/>
-              <a:satMod val="130000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="80000">
-            <a:schemeClr val="phClr">
-              <a:shade val="93000"/>
-              <a:satMod val="130000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:shade val="94000"/>
-              <a:satMod val="135000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="16200000" scaled="0"/>
-      </a:gradFill>
-    </a:fillStyleLst>
-    <a:lnStyleLst>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-            <a:satMod val="105000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-      </a:ln>
-      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-      </a:ln>
-      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="solid"/>
-      </a:ln>
-    </a:lnStyleLst>
-    <a:effectStyleLst>
-      <a:effectStyle>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </a:effectStyle>
-      <a:effectStyle>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </a:effectStyle>
-      <a:effectStyle>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront">
-            <a:rot lat="0" lon="0" rev="0"/>
-          </a:camera>
-          <a:lightRig rig="threePt" dir="t">
-            <a:rot lat="0" lon="0" rev="1200000"/>
-          </a:lightRig>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="63500" h="25400"/>
-        </a:sp3d>
-      </a:effectStyle>
-    </a:effectStyleLst>
-    <a:bgFillStyleLst>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:tint val="40000"/>
-              <a:satMod val="350000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="40000">
-            <a:schemeClr val="phClr">
-              <a:tint val="45000"/>
-              <a:shade val="99000"/>
-              <a:satMod val="350000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:shade val="20000"/>
-              <a:satMod val="255000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-      </a:gradFill>
-      <a:gradFill rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr">
-              <a:tint val="80000"/>
-              <a:satMod val="300000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:shade val="30000"/>
-              <a:satMod val="200000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-      </a:gradFill>
-    </a:bgFillStyleLst>
-  </a:fmtScheme>
-</a:themeOverride>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34:J41"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5363,7 +4786,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -5445,7 +4868,7 @@
         <v>2.7440710539815454</v>
       </c>
     </row>
-    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -5508,7 +4931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -5571,7 +4994,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -5634,7 +5057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -5681,7 +5104,7 @@
         <v>4.2559289460184546</v>
       </c>
     </row>
-    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -5709,7 +5132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -5737,7 +5160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -5780,7 +5203,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -5858,7 +5281,7 @@
         <v>2.1906926585840458</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -5920,7 +5343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -5982,7 +5405,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -6045,7 +5468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5</v>
       </c>
@@ -6092,7 +5515,7 @@
         <v>4.8093073414159537</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -6120,7 +5543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -6148,7 +5571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8</v>
       </c>
@@ -6592,7 +6015,7 @@
   <autoFilter ref="A1:J49">
     <filterColumn colId="1">
       <filters>
-        <filter val="5"/>
+        <filter val="4"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -7281,8 +6704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>